<commit_message>
Actualización textos sitio internacional
</commit_message>
<xml_diff>
--- a/Archivos CSV/Inventory Location/inventory_location template site_Maaji.xlsx
+++ b/Archivos CSV/Inventory Location/inventory_location template site_Maaji.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvargasp\Documents\Commerce-Conect-FF\Archivos CSV\Inventory Location\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvargasp\Documents\Archivos MAAJI\Archivos CSV\Inventory Location\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E6DFB8-3CDF-46B8-A94D-DD657C8560E3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8289BE-062C-4ED1-BCA5-637F405EB1D2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{F1F2D59A-6786-4EBD-AB3D-AB089D2830A2}"/>
   </bookViews>
@@ -371,6 +371,30 @@
     <t>110211</t>
   </si>
   <si>
+    <t>Maaji_Retiro_co</t>
+  </si>
+  <si>
+    <t>Maaji_Barranquilla_co</t>
+  </si>
+  <si>
+    <t>Maaji_Cartagena_co</t>
+  </si>
+  <si>
+    <t>Maaji_Tesoro_co</t>
+  </si>
+  <si>
+    <t>Maaji_Cali_co</t>
+  </si>
+  <si>
+    <t>Maaji_Bocagrande_co</t>
+  </si>
+  <si>
+    <t>Maaji_Santafe_co</t>
+  </si>
+  <si>
+    <t>Maaji_Bucaramanga_co</t>
+  </si>
+  <si>
     <t>business_hour.1.day_name</t>
   </si>
   <si>
@@ -483,37 +507,13 @@
   </si>
   <si>
     <t>site_Maaji</t>
-  </si>
-  <si>
-    <t>Maaji_Retiro</t>
-  </si>
-  <si>
-    <t>Maaji_Barranquilla</t>
-  </si>
-  <si>
-    <t>Maaji_Cartagena</t>
-  </si>
-  <si>
-    <t>Maaji_Tesoro</t>
-  </si>
-  <si>
-    <t>Maaji_Cali</t>
-  </si>
-  <si>
-    <t>Maaji_Bocagrande</t>
-  </si>
-  <si>
-    <t>Maaji_Santafe</t>
-  </si>
-  <si>
-    <t>Maaji_Bucaramanga</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,316 +521,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -838,207 +538,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1356,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774A88B6-025C-4213-9962-8FA505AD9F0D}">
   <dimension ref="A1:AZ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1002,7 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="AA1" t="s">
         <v>25</v>
@@ -1504,7 +1014,7 @@
         <v>27</v>
       </c>
       <c r="AD1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="AE1" t="s">
         <v>28</v>
@@ -1516,7 +1026,7 @@
         <v>30</v>
       </c>
       <c r="AH1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="AI1" t="s">
         <v>31</v>
@@ -1528,7 +1038,7 @@
         <v>33</v>
       </c>
       <c r="AL1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="AM1" t="s">
         <v>34</v>
@@ -1540,7 +1050,7 @@
         <v>36</v>
       </c>
       <c r="AP1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="AQ1" t="s">
         <v>37</v>
@@ -1552,7 +1062,7 @@
         <v>39</v>
       </c>
       <c r="AT1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="AU1" t="s">
         <v>40</v>
@@ -1564,7 +1074,7 @@
         <v>42</v>
       </c>
       <c r="AX1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="AY1" t="s">
         <v>43</v>
@@ -1577,8 +1087,8 @@
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>133</v>
+      <c r="B2" t="s">
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
@@ -1605,22 +1115,22 @@
         <v>52</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="P2" t="s">
         <v>53</v>
       </c>
       <c r="V2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="Y2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Z2" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AA2" s="1">
         <v>0.41666666666666669</v>
@@ -1629,10 +1139,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AC2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="AD2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="AE2" s="1">
         <v>0.41666666666666669</v>
@@ -1641,10 +1151,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AG2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="AH2" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="AI2" s="1">
         <v>0.41666666666666669</v>
@@ -1653,10 +1163,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AK2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="AL2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="AM2" s="1">
         <v>0.41666666666666669</v>
@@ -1665,10 +1175,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AO2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AP2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AQ2" s="1">
         <v>0.41666666666666669</v>
@@ -1677,10 +1187,10 @@
         <v>0.875</v>
       </c>
       <c r="AS2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AT2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AU2" s="1">
         <v>0.41666666666666669</v>
@@ -1689,10 +1199,10 @@
         <v>0.875</v>
       </c>
       <c r="AW2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="AX2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AY2" s="1">
         <v>0.5</v>
@@ -1705,8 +1215,8 @@
       <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>134</v>
+      <c r="B3" t="s">
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>55</v>
@@ -1733,22 +1243,22 @@
         <v>52</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="P3">
         <v>3234886286</v>
       </c>
       <c r="V3" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="Y3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Z3" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AA3" s="1">
         <v>0.41666666666666669</v>
@@ -1757,23 +1267,23 @@
         <v>0.875</v>
       </c>
       <c r="AC3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH3" t="s">
         <v>113</v>
       </c>
-      <c r="AD3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>0.875</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>105</v>
-      </c>
       <c r="AI3" s="1">
         <v>0.41666666666666669</v>
       </c>
@@ -1781,10 +1291,10 @@
         <v>0.875</v>
       </c>
       <c r="AK3" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="AL3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="AM3" s="1">
         <v>0.41666666666666669</v>
@@ -1793,10 +1303,10 @@
         <v>0.875</v>
       </c>
       <c r="AO3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AP3" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AQ3" s="1">
         <v>0.41666666666666669</v>
@@ -1805,10 +1315,10 @@
         <v>0.875</v>
       </c>
       <c r="AS3" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AT3" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AU3" s="1">
         <v>0.41666666666666669</v>
@@ -1817,10 +1327,10 @@
         <v>0.875</v>
       </c>
       <c r="AW3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="AX3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AY3" s="1">
         <v>0.45833333333333331</v>
@@ -1833,8 +1343,8 @@
       <c r="A4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>135</v>
+      <c r="B4" t="s">
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>61</v>
@@ -1861,22 +1371,22 @@
         <v>52</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="P4">
         <v>6643079</v>
       </c>
       <c r="V4" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="Y4" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Z4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AA4" s="1">
         <v>0.41666666666666669</v>
@@ -1885,23 +1395,23 @@
         <v>0.875</v>
       </c>
       <c r="AC4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH4" t="s">
         <v>113</v>
       </c>
-      <c r="AD4" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE4" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="AF4" s="1">
-        <v>0.875</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>105</v>
-      </c>
       <c r="AI4" s="1">
         <v>0.41666666666666669</v>
       </c>
@@ -1909,10 +1419,10 @@
         <v>0.875</v>
       </c>
       <c r="AK4" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="AL4" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="AM4" s="1">
         <v>0.41666666666666669</v>
@@ -1921,10 +1431,10 @@
         <v>0.875</v>
       </c>
       <c r="AO4" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AP4" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AQ4" s="1">
         <v>0.41666666666666669</v>
@@ -1933,10 +1443,10 @@
         <v>0.875</v>
       </c>
       <c r="AS4" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AT4" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AU4" s="1">
         <v>0.41666666666666669</v>
@@ -1945,10 +1455,10 @@
         <v>0.875</v>
       </c>
       <c r="AW4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="AX4" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AY4" s="1">
         <v>0.45833333333333331</v>
@@ -1961,8 +1471,8 @@
       <c r="A5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>136</v>
+      <c r="B5" t="s">
+        <v>98</v>
       </c>
       <c r="C5" t="s">
         <v>66</v>
@@ -1989,22 +1499,22 @@
         <v>52</v>
       </c>
       <c r="M5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="P5" t="s">
         <v>71</v>
       </c>
       <c r="V5" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="Y5" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Z5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AA5" s="1">
         <v>0.41666666666666669</v>
@@ -2013,23 +1523,23 @@
         <v>0.875</v>
       </c>
       <c r="AC5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH5" t="s">
         <v>113</v>
       </c>
-      <c r="AD5" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE5" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="AF5" s="1">
-        <v>0.875</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>105</v>
-      </c>
       <c r="AI5" s="1">
         <v>0.41666666666666669</v>
       </c>
@@ -2037,10 +1547,10 @@
         <v>0.875</v>
       </c>
       <c r="AK5" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="AL5" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="AM5" s="1">
         <v>0.41666666666666669</v>
@@ -2049,10 +1559,10 @@
         <v>0.875</v>
       </c>
       <c r="AO5" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AP5" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AQ5" s="1">
         <v>0.41666666666666669</v>
@@ -2061,10 +1571,10 @@
         <v>0.875</v>
       </c>
       <c r="AS5" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AT5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AU5" s="1">
         <v>0.41666666666666669</v>
@@ -2073,10 +1583,10 @@
         <v>0.875</v>
       </c>
       <c r="AW5" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="AX5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AY5" s="1">
         <v>0.45833333333333331</v>
@@ -2089,8 +1599,8 @@
       <c r="A6" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>137</v>
+      <c r="B6" t="s">
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>73</v>
@@ -2117,22 +1627,22 @@
         <v>52</v>
       </c>
       <c r="M6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="P6">
         <v>3481149</v>
       </c>
       <c r="V6" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="Y6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Z6" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AA6" s="1">
         <v>0.41666666666666669</v>
@@ -2141,10 +1651,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AC6" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="AD6" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="AE6" s="1">
         <v>0.41666666666666669</v>
@@ -2153,10 +1663,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AG6" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="AH6" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="AI6" s="1">
         <v>0.41666666666666669</v>
@@ -2165,10 +1675,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AK6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="AL6" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="AM6" s="1">
         <v>0.41666666666666669</v>
@@ -2177,10 +1687,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AO6" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AP6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AQ6" s="1">
         <v>0.41666666666666669</v>
@@ -2189,10 +1699,10 @@
         <v>0.875</v>
       </c>
       <c r="AS6" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AT6" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AU6" s="1">
         <v>0.41666666666666669</v>
@@ -2201,10 +1711,10 @@
         <v>0.875</v>
       </c>
       <c r="AW6" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="AX6" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AY6" s="1">
         <v>0.45833333333333331</v>
@@ -2217,8 +1727,8 @@
       <c r="A7" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>138</v>
+      <c r="B7" t="s">
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>79</v>
@@ -2245,22 +1755,22 @@
         <v>52</v>
       </c>
       <c r="M7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="P7">
         <v>3205600544</v>
       </c>
       <c r="V7" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="Y7" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Z7" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AA7" s="1">
         <v>0.41666666666666669</v>
@@ -2269,10 +1779,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AC7" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="AD7" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="AE7" s="1">
         <v>0.41666666666666669</v>
@@ -2281,10 +1791,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AG7" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="AH7" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="AI7" s="1">
         <v>0.41666666666666669</v>
@@ -2293,10 +1803,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AK7" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="AL7" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="AM7" s="1">
         <v>0.41666666666666669</v>
@@ -2305,10 +1815,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AO7" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AP7" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AQ7" s="1">
         <v>0.41666666666666669</v>
@@ -2317,10 +1827,10 @@
         <v>0.875</v>
       </c>
       <c r="AS7" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AT7" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AU7" s="1">
         <v>0.41666666666666669</v>
@@ -2329,10 +1839,10 @@
         <v>0.875</v>
       </c>
       <c r="AW7" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="AX7" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AY7" s="1">
         <v>0.41666666666666669</v>
@@ -2345,8 +1855,8 @@
       <c r="A8" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>139</v>
+      <c r="B8" t="s">
+        <v>101</v>
       </c>
       <c r="C8" t="s">
         <v>83</v>
@@ -2373,22 +1883,22 @@
         <v>52</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="P8">
         <v>3173649859</v>
       </c>
       <c r="V8" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="Y8" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Z8" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AA8" s="1">
         <v>0.41666666666666669</v>
@@ -2397,23 +1907,23 @@
         <v>0.875</v>
       </c>
       <c r="AC8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH8" t="s">
         <v>113</v>
       </c>
-      <c r="AD8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE8" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="AF8" s="1">
-        <v>0.875</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>105</v>
-      </c>
       <c r="AI8" s="1">
         <v>0.41666666666666669</v>
       </c>
@@ -2421,10 +1931,10 @@
         <v>0.875</v>
       </c>
       <c r="AK8" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="AL8" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="AM8" s="1">
         <v>0.41666666666666669</v>
@@ -2433,10 +1943,10 @@
         <v>0.875</v>
       </c>
       <c r="AO8" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AP8" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AQ8" s="1">
         <v>0.41666666666666669</v>
@@ -2445,10 +1955,10 @@
         <v>0.875</v>
       </c>
       <c r="AS8" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AT8" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AU8" s="1">
         <v>0.41666666666666669</v>
@@ -2457,10 +1967,10 @@
         <v>0.875</v>
       </c>
       <c r="AW8" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="AX8" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AY8" s="1">
         <v>0.45833333333333331</v>
@@ -2473,8 +1983,8 @@
       <c r="A9" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>140</v>
+      <c r="B9" t="s">
+        <v>102</v>
       </c>
       <c r="C9" t="s">
         <v>87</v>
@@ -2501,22 +2011,22 @@
         <v>52</v>
       </c>
       <c r="M9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="P9">
         <v>4488870</v>
       </c>
       <c r="V9" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="Y9" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="Z9" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="AA9" s="1">
         <v>0.41666666666666669</v>
@@ -2525,10 +2035,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AC9" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="AD9" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="AE9" s="1">
         <v>0.41666666666666669</v>
@@ -2537,10 +2047,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AG9" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="AH9" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="AI9" s="1">
         <v>0.41666666666666669</v>
@@ -2549,10 +2059,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AK9" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="AL9" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="AM9" s="1">
         <v>0.41666666666666669</v>
@@ -2561,10 +2071,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AO9" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AP9" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="AQ9" s="1">
         <v>0.41666666666666669</v>
@@ -2573,10 +2083,10 @@
         <v>0.875</v>
       </c>
       <c r="AS9" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="AT9" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="AU9" s="1">
         <v>0.41666666666666669</v>
@@ -2585,10 +2095,10 @@
         <v>0.875</v>
       </c>
       <c r="AW9" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="AX9" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AY9" s="1">
         <v>0.41666666666666669</v>

</xml_diff>